<commit_message>
ca assay compiled data
</commit_message>
<xml_diff>
--- a/Hemolymph_Calcium_Assay/data/20201125/CompiledData.xlsx
+++ b/Hemolymph_Calcium_Assay/data/20201125/CompiledData.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/HHD/Documents/GitHub/P_generosa/Hemolymph_Calcium_Assay/data/20201125/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFBC0DE4-8370-7447-AFD9-D49E0EE808D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B5EA44C-436F-F040-B901-7CEF871619E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6660" yWindow="460" windowWidth="21060" windowHeight="13380" xr2:uid="{754D4AD5-624D-8D44-8D68-36FE97CADD15}"/>
+    <workbookView xWindow="4540" yWindow="460" windowWidth="21060" windowHeight="13380" xr2:uid="{754D4AD5-624D-8D44-8D68-36FE97CADD15}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="CompiledData" sheetId="1" r:id="rId1"/>
+    <sheet name="STDs" sheetId="3" r:id="rId2"/>
+    <sheet name="PlateMap" sheetId="2" r:id="rId3"/>
     <sheet name="SampleInfo" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029" iterate="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1927" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2013" uniqueCount="265">
   <si>
     <t>Plate</t>
   </si>
@@ -829,6 +829,9 @@
   <si>
     <t>01/23-040L</t>
   </si>
+  <si>
+    <t>Sex</t>
+  </si>
 </sst>
 </file>
 
@@ -1028,7 +1031,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$9:$A$16</c:f>
+              <c:f>STDs!$A$9:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1061,7 +1064,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$E$9:$E$16</c:f>
+              <c:f>STDs!$E$9:$E$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1412,7 +1415,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$1:$A$8</c:f>
+              <c:f>STDs!$A$1:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1445,7 +1448,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$E$1:$E$8</c:f>
+              <c:f>STDs!$E$1:$E$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1818,7 +1821,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$17:$A$24</c:f>
+              <c:f>STDs!$A$17:$A$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1851,7 +1854,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$E$17:$E$24</c:f>
+              <c:f>STDs!$E$17:$E$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2224,7 +2227,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet3!$A$25:$A$32</c:f>
+              <c:f>STDs!$A$25:$A$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2257,7 +2260,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet3!$E$25:$E$32</c:f>
+              <c:f>STDs!$E$25:$E$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -4602,8 +4605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E4D1614-62BF-384D-B2B6-7BC9CDBFEE94}">
   <dimension ref="A1:N385"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A137" workbookViewId="0">
-      <selection activeCell="H160" sqref="H160"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H102" sqref="H102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -13486,7 +13489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E52BAB6B-2D63-2248-9589-662D53E1E5E8}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView zoomScale="190" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScale="75" workbookViewId="0">
       <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
@@ -42969,15 +42972,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4946A411-0CFF-8649-8F41-9892A6DA466B}">
-  <dimension ref="A1:E86"/>
+  <dimension ref="A1:J86"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>210</v>
       </c>
@@ -42993,8 +42996,11 @@
       <c r="E1" s="4" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="4" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>20181119</v>
       </c>
@@ -43010,8 +43016,14 @@
       <c r="E2" s="4" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>20190104</v>
       </c>
@@ -43027,8 +43039,14 @@
       <c r="E3" s="4" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>20190123</v>
       </c>
@@ -43044,8 +43062,14 @@
       <c r="E4" s="4" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>20181119</v>
       </c>
@@ -43061,8 +43085,14 @@
       <c r="E5" s="4" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
         <v>20190104</v>
       </c>
@@ -43078,8 +43108,14 @@
       <c r="E6" s="4" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>20190221</v>
       </c>
@@ -43095,8 +43131,14 @@
       <c r="E7" s="4" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="4">
         <v>20181119</v>
       </c>
@@ -43112,8 +43154,14 @@
       <c r="E8" s="4" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>20190104</v>
       </c>
@@ -43129,8 +43177,14 @@
       <c r="E9" s="4" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="4">
         <v>20190221</v>
       </c>
@@ -43146,8 +43200,14 @@
       <c r="E10" s="4" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="4">
         <v>20181119</v>
       </c>
@@ -43163,8 +43223,14 @@
       <c r="E11" s="4" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="4">
         <v>20190104</v>
       </c>
@@ -43180,8 +43246,14 @@
       <c r="E12" s="4" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="4">
         <v>20190221</v>
       </c>
@@ -43197,8 +43269,14 @@
       <c r="E13" s="4" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="4">
         <v>20181119</v>
       </c>
@@ -43214,8 +43292,14 @@
       <c r="E14" s="4" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>20190104</v>
       </c>
@@ -43231,8 +43315,14 @@
       <c r="E15" s="4" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="4">
         <v>20190123</v>
       </c>
@@ -43248,8 +43338,14 @@
       <c r="E16" s="4" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="4">
         <v>20181119</v>
       </c>
@@ -43265,8 +43361,14 @@
       <c r="E17" s="4" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="4">
         <v>20190104</v>
       </c>
@@ -43282,8 +43384,14 @@
       <c r="E18" s="4" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="4">
         <v>20190221</v>
       </c>
@@ -43299,8 +43407,14 @@
       <c r="E19" s="4" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>20181119</v>
       </c>
@@ -43316,8 +43430,14 @@
       <c r="E20" s="4" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="4">
         <v>20190104</v>
       </c>
@@ -43333,8 +43453,14 @@
       <c r="E21" s="4" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="4">
         <v>20190123</v>
       </c>
@@ -43350,8 +43476,14 @@
       <c r="E22" s="4" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="4">
         <v>20181119</v>
       </c>
@@ -43367,8 +43499,14 @@
       <c r="E23" s="4" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="4">
         <v>20190104</v>
       </c>
@@ -43384,8 +43522,14 @@
       <c r="E24" s="4" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="4">
         <v>20190123</v>
       </c>
@@ -43401,8 +43545,14 @@
       <c r="E25" s="4" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="4">
         <v>20181119</v>
       </c>
@@ -43418,8 +43568,14 @@
       <c r="E26" s="4" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="4">
         <v>20190104</v>
       </c>
@@ -43435,8 +43591,14 @@
       <c r="E27" s="4" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="4">
         <v>20190221</v>
       </c>
@@ -43452,8 +43614,14 @@
       <c r="E28" s="4" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="4">
         <v>20181119</v>
       </c>
@@ -43469,8 +43637,14 @@
       <c r="E29" s="4" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>20190104</v>
       </c>
@@ -43486,8 +43660,14 @@
       <c r="E30" s="4" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
         <v>20190123</v>
       </c>
@@ -43503,8 +43683,14 @@
       <c r="E31" s="4" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="4">
         <v>20181119</v>
       </c>
@@ -43520,8 +43706,14 @@
       <c r="E32" s="4" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="4">
         <v>20190104</v>
       </c>
@@ -43537,8 +43729,14 @@
       <c r="E33" s="4" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="4">
         <v>20190123</v>
       </c>
@@ -43554,8 +43752,14 @@
       <c r="E34" s="4" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="4">
         <v>20181119</v>
       </c>
@@ -43571,8 +43775,14 @@
       <c r="E35" s="4" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="4">
         <v>20190104</v>
       </c>
@@ -43588,8 +43798,14 @@
       <c r="E36" s="4" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="4">
         <v>20190221</v>
       </c>
@@ -43605,8 +43821,14 @@
       <c r="E37" s="4" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="4">
         <v>20181119</v>
       </c>
@@ -43622,8 +43844,14 @@
       <c r="E38" s="4" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="4">
         <v>20190104</v>
       </c>
@@ -43639,8 +43867,14 @@
       <c r="E39" s="4" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="4">
         <v>20190221</v>
       </c>
@@ -43656,8 +43890,14 @@
       <c r="E40" s="4" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F40" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="2"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="4">
         <v>20181119</v>
       </c>
@@ -43673,8 +43913,14 @@
       <c r="E41" s="4" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F41" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="4">
         <v>20190104</v>
       </c>
@@ -43690,8 +43936,14 @@
       <c r="E42" s="4" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F42" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2"/>
+      <c r="J42" s="2"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="4">
         <v>20190123</v>
       </c>
@@ -43707,8 +43959,14 @@
       <c r="E43" s="4" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F43" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
         <v>20181119</v>
       </c>
@@ -43724,8 +43982,14 @@
       <c r="E44" s="4" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F44" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="J44" s="2"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="4">
         <v>20190104</v>
       </c>
@@ -43741,8 +44005,14 @@
       <c r="E45" s="4" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F45" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="J45" s="2"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="4">
         <v>20190123</v>
       </c>
@@ -43758,8 +44028,11 @@
       <c r="E46" s="4" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F46" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="4">
         <v>20181119</v>
       </c>
@@ -43775,8 +44048,11 @@
       <c r="E47" s="4" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F47" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="4">
         <v>20190104</v>
       </c>
@@ -43792,8 +44068,11 @@
       <c r="E48" s="4" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F48" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="4">
         <v>20190221</v>
       </c>
@@ -43809,8 +44088,11 @@
       <c r="E49" s="4" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F49" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="4">
         <v>20181119</v>
       </c>
@@ -43826,8 +44108,11 @@
       <c r="E50" s="4" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F50" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="4">
         <v>20190104</v>
       </c>
@@ -43843,8 +44128,11 @@
       <c r="E51" s="4" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F51" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="4">
         <v>20190123</v>
       </c>
@@ -43860,8 +44148,11 @@
       <c r="E52" s="4" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F52" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="4">
         <v>20181119</v>
       </c>
@@ -43877,8 +44168,11 @@
       <c r="E53" s="4" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F53" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="4">
         <v>20190104</v>
       </c>
@@ -43894,8 +44188,11 @@
       <c r="E54" s="4" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F54" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="4">
         <v>20190123</v>
       </c>
@@ -43911,8 +44208,11 @@
       <c r="E55" s="4" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F55" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="4">
         <v>20181119</v>
       </c>
@@ -43928,8 +44228,11 @@
       <c r="E56" s="4" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F56" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="4">
         <v>20190104</v>
       </c>
@@ -43945,8 +44248,11 @@
       <c r="E57" s="4" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F57" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="4">
         <v>20190221</v>
       </c>
@@ -43962,8 +44268,11 @@
       <c r="E58" s="4" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F58" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="4">
         <v>20181119</v>
       </c>
@@ -43979,8 +44288,11 @@
       <c r="E59" s="4" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F59" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="4">
         <v>20190104</v>
       </c>
@@ -43996,8 +44308,11 @@
       <c r="E60" s="4" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F60" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="4">
         <v>20190221</v>
       </c>
@@ -44013,8 +44328,11 @@
       <c r="E61" s="4" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F61" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="4">
         <v>20181119</v>
       </c>
@@ -44030,8 +44348,11 @@
       <c r="E62" s="4" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F62" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="4">
         <v>20190104</v>
       </c>
@@ -44047,8 +44368,11 @@
       <c r="E63" s="4" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F63" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="4">
         <v>20190221</v>
       </c>
@@ -44064,8 +44388,11 @@
       <c r="E64" s="4" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F64" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="4">
         <v>20190123</v>
       </c>
@@ -44081,8 +44408,11 @@
       <c r="E65" s="4" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F65" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="4">
         <v>20190123</v>
       </c>
@@ -44098,8 +44428,11 @@
       <c r="E66" s="4" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F66" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="4">
         <v>20190123</v>
       </c>
@@ -44115,8 +44448,11 @@
       <c r="E67" s="4" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F67" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="4">
         <v>20190123</v>
       </c>
@@ -44132,8 +44468,11 @@
       <c r="E68" s="4" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F68" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="4">
         <v>20190123</v>
       </c>
@@ -44149,8 +44488,11 @@
       <c r="E69" s="4" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F69" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="4">
         <v>20190123</v>
       </c>
@@ -44166,8 +44508,11 @@
       <c r="E70" s="4" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F70" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="4">
         <v>20190123</v>
       </c>
@@ -44183,8 +44528,11 @@
       <c r="E71" s="4" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F71" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="4">
         <v>20190123</v>
       </c>
@@ -44200,8 +44548,11 @@
       <c r="E72" s="4" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F72" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="4">
         <v>20190123</v>
       </c>
@@ -44217,8 +44568,11 @@
       <c r="E73" s="4" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F73" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="4">
         <v>20190221</v>
       </c>
@@ -44234,8 +44588,11 @@
       <c r="E74" s="4" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F74" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="4">
         <v>20190221</v>
       </c>
@@ -44251,8 +44608,11 @@
       <c r="E75" s="4" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F75" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="4">
         <v>20190221</v>
       </c>
@@ -44268,8 +44628,11 @@
       <c r="E76" s="4" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F76" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="4">
         <v>20190221</v>
       </c>
@@ -44285,8 +44648,11 @@
       <c r="E77" s="4" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F77" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="4">
         <v>20190221</v>
       </c>
@@ -44302,8 +44668,11 @@
       <c r="E78" s="4" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F78" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="4">
         <v>20190221</v>
       </c>
@@ -44319,8 +44688,11 @@
       <c r="E79" s="4" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F79" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="4">
         <v>20190221</v>
       </c>
@@ -44336,8 +44708,11 @@
       <c r="E80" s="4" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F80" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="4">
         <v>20190221</v>
       </c>
@@ -44353,8 +44728,11 @@
       <c r="E81" s="4" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F81" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="4">
         <v>20190221</v>
       </c>
@@ -44370,8 +44748,11 @@
       <c r="E82" s="4" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F82" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="4">
         <v>20190221</v>
       </c>
@@ -44387,8 +44768,11 @@
       <c r="E83" s="4" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F83" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="4">
         <v>20190221</v>
       </c>
@@ -44404,8 +44788,11 @@
       <c r="E84" s="4" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F84" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="4">
         <v>20190221</v>
       </c>
@@ -44421,8 +44808,11 @@
       <c r="E85" s="4" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F85" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="4">
         <v>20190221</v>
       </c>
@@ -44438,8 +44828,14 @@
       <c r="E86" s="4" t="s">
         <v>262</v>
       </c>
+      <c r="F86" s="4" t="s">
+        <v>129</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H2:J45">
+    <sortCondition ref="I2:I45"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>